<commit_message>
Changed excel doc to include totals.
</commit_message>
<xml_diff>
--- a/explorecoursesassessment.xlsx
+++ b/explorecoursesassessment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>explore course</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>ours</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -132,8 +135,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -143,9 +150,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -723,6 +734,19 @@
       </c>
       <c r="H22">
         <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24">
+        <f>SUM(G2:G22)</f>
+        <v>750</v>
+      </c>
+      <c r="H24">
+        <f>SUM(H2:H22)</f>
+        <v>1390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote results section in final report.
</commit_message>
<xml_diff>
--- a/explorecoursesassessment.xlsx
+++ b/explorecoursesassessment.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>explore course</t>
   </si>
@@ -135,8 +136,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -150,13 +197,59 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,7 +582,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -532,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H4">
         <v>60</v>
@@ -590,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>100</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="12">
@@ -667,7 +760,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="12">
@@ -742,11 +835,11 @@
       </c>
       <c r="G24">
         <f>SUM(G2:G22)</f>
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="H24">
         <f>SUM(H2:H22)</f>
-        <v>1390</v>
+        <v>1290</v>
       </c>
     </row>
   </sheetData>
@@ -762,4 +855,276 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A9:H75"/>
+  <sheetViews>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="48">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="36">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29">
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34">
+        <v>100</v>
+      </c>
+      <c r="H34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="G35">
+        <f>SUM(G25:G34)</f>
+        <v>300</v>
+      </c>
+      <c r="H35">
+        <f>SUM(H25:H34)</f>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>100</v>
+      </c>
+      <c r="H70">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71">
+        <v>100</v>
+      </c>
+      <c r="H71">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="G72">
+        <v>100</v>
+      </c>
+      <c r="H72">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74">
+        <v>100</v>
+      </c>
+      <c r="H74">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="G75">
+        <f>SUM(G70:G74)</f>
+        <v>400</v>
+      </c>
+      <c r="H75">
+        <f>SUM(H70:H74)</f>
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>